<commit_message>
coursearrange: Add fucntions for course arrange by admin
</commit_message>
<xml_diff>
--- a/resources/test/智慧教室测试数据.xlsx
+++ b/resources/test/智慧教室测试数据.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16828"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="课程" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="89">
   <si>
     <t>未使用</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -341,13 +341,33 @@
   </si>
   <si>
     <t>herry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>80课时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4课时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8课时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>60课时</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100课时</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -425,7 +445,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -500,6 +520,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -535,6 +572,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -713,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -777,6 +831,9 @@
       <c r="G2" t="s">
         <v>58</v>
       </c>
+      <c r="H2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
@@ -797,6 +854,9 @@
       <c r="G3" t="s">
         <v>21</v>
       </c>
+      <c r="H3" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
@@ -817,6 +877,9 @@
       <c r="G4" t="s">
         <v>22</v>
       </c>
+      <c r="H4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
@@ -837,6 +900,9 @@
       <c r="G5" t="s">
         <v>59</v>
       </c>
+      <c r="H5" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
@@ -977,6 +1043,9 @@
       <c r="G12" t="s">
         <v>21</v>
       </c>
+      <c r="H12" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
@@ -994,6 +1063,9 @@
       <c r="E13" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="H13" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
@@ -1007,6 +1079,9 @@
       </c>
       <c r="E14" s="2" t="s">
         <v>46</v>
+      </c>
+      <c r="H14" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1025,7 +1100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>

<commit_message>
Course Choose: Add for student course choose function
</commit_message>
<xml_diff>
--- a/resources/test/智慧教室测试数据.xlsx
+++ b/resources/test/智慧教室测试数据.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="87">
   <si>
     <t>未使用</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -196,14 +196,6 @@
     <t>每天</t>
   </si>
   <si>
-    <t>星期三第3,4节</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>星期四第1,2节</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>星期二第5,6节</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -344,23 +336,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>80课时</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4课时</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8课时</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>60课时</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100课时</t>
+    <t>人数(Studnums)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>课时(Coursenums)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>星期三第3,4节 星期五第1,2节</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>星期二第3,4节 星期四第1,2节</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>星期二第5,6节 星期四第7,8节</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -765,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -776,40 +768,43 @@
     <col min="1" max="1" width="12.75" customWidth="1"/>
     <col min="2" max="2" width="21.375" customWidth="1"/>
     <col min="3" max="3" width="11.375" customWidth="1"/>
-    <col min="4" max="4" width="23.625" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
     <col min="5" max="5" width="14.625" customWidth="1"/>
     <col min="6" max="6" width="11.375" customWidth="1"/>
     <col min="7" max="7" width="15.75" customWidth="1"/>
-    <col min="8" max="8" width="18.25" customWidth="1"/>
+    <col min="8" max="9" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+        <v>82</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -820,22 +815,25 @@
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+        <v>56</v>
+      </c>
+      <c r="H2">
+        <v>40</v>
+      </c>
+      <c r="I2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -846,7 +844,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>43</v>
@@ -854,11 +852,14 @@
       <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="H3">
+        <v>40</v>
+      </c>
+      <c r="I3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -869,7 +870,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>43</v>
@@ -877,11 +878,14 @@
       <c r="G4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="H4">
+        <v>60</v>
+      </c>
+      <c r="I4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -892,19 +896,22 @@
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+        <v>57</v>
+      </c>
+      <c r="H5">
+        <v>60</v>
+      </c>
+      <c r="I5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -915,16 +922,16 @@
         <v>6</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -935,16 +942,16 @@
         <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -955,16 +962,16 @@
         <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -975,16 +982,16 @@
         <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -995,16 +1002,16 @@
         <v>15</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1015,16 +1022,16 @@
         <v>15</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1035,7 +1042,7 @@
         <v>7</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>43</v>
@@ -1043,11 +1050,11 @@
       <c r="G12" t="s">
         <v>21</v>
       </c>
-      <c r="H12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1058,16 +1065,16 @@
         <v>31</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1075,13 +1082,13 @@
         <v>45</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H14" t="s">
-        <v>86</v>
+      <c r="I14">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1116,28 +1123,28 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
@@ -1214,7 +1221,7 @@
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G5" t="s">
         <v>1</v>
@@ -1237,7 +1244,7 @@
         <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G6" t="s">
         <v>1</v>

</xml_diff>